<commit_message>
fix: make templates business-agnostic — replace specific names with generic slots
Templates previously used business-specific sheet names (ミールモデル,
アカデミーモデル, コンサルモデル) that contaminated LLM analysis for
any non-matching business. Replaced with generic numbered slots
(収益モデル1, 収益モデル2, 収益モデル3) and cleaned all corresponding
references from agent prompts.

https://claude.ai/code/session_01Q6zXhRH3pSwH7bCCx5FC45
</commit_message>
<xml_diff>
--- a/templates/base.xlsx
+++ b/templates/base.xlsx
@@ -8,9 +8,9 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PL設計" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ミールモデル" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="アカデミーモデル" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="コンサルモデル" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="収益モデル1" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="収益モデル2" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="収益モデル3" sheetId="4" state="visible" r:id="rId4"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="費用まとめ" sheetId="5" state="visible" r:id="rId5"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="費用リスト" sheetId="6" state="visible" r:id="rId6"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="費用タグ" sheetId="7" state="visible" r:id="rId7"/>
@@ -618,23 +618,23 @@
         </is>
       </c>
       <c r="B4" s="5">
-        <f>'ミールモデル'!B10+'アカデミーモデル'!B10+'コンサルモデル'!B10</f>
+        <f>'収益モデル1'!B10+'収益モデル2'!B10+'収益モデル3'!B10</f>
         <v/>
       </c>
       <c r="C4" s="5">
-        <f>'ミールモデル'!C10+'アカデミーモデル'!C10+'コンサルモデル'!C10</f>
+        <f>'収益モデル1'!C10+'収益モデル2'!C10+'収益モデル3'!C10</f>
         <v/>
       </c>
       <c r="D4" s="5">
-        <f>'ミールモデル'!D10+'アカデミーモデル'!D10+'コンサルモデル'!D10</f>
+        <f>'収益モデル1'!D10+'収益モデル2'!D10+'収益モデル3'!D10</f>
         <v/>
       </c>
       <c r="E4" s="5">
-        <f>'ミールモデル'!E10+'アカデミーモデル'!E10+'コンサルモデル'!E10</f>
+        <f>'収益モデル1'!E10+'収益モデル2'!E10+'収益モデル3'!E10</f>
         <v/>
       </c>
       <c r="F4" s="5">
-        <f>'ミールモデル'!F10+'アカデミーモデル'!F10+'コンサルモデル'!F10</f>
+        <f>'収益モデル1'!F10+'収益モデル2'!F10+'収益モデル3'!F10</f>
         <v/>
       </c>
     </row>
@@ -889,7 +889,7 @@
     <row r="1" ht="30" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>ミールモデル（ユニットエコノミクス）</t>
+          <t>収益モデル1（セグメント1）</t>
         </is>
       </c>
     </row>
@@ -924,7 +924,7 @@
     <row r="3">
       <c r="A3" s="6" t="inlineStr">
         <is>
-          <t>顧客数</t>
+          <t>顧客数/取引数</t>
         </is>
       </c>
       <c r="B3" s="14" t="n">
@@ -934,19 +934,19 @@
         <v>200</v>
       </c>
       <c r="D3" s="14" t="n">
-        <v>350</v>
+        <v>360</v>
       </c>
       <c r="E3" s="14" t="n">
-        <v>500</v>
+        <v>560</v>
       </c>
       <c r="F3" s="14" t="n">
-        <v>700</v>
+        <v>800</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="6" t="inlineStr">
         <is>
-          <t>客単価（円/月）</t>
+          <t>単価（円）</t>
         </is>
       </c>
       <c r="B4" s="14" t="n">
@@ -956,26 +956,26 @@
         <v>5000</v>
       </c>
       <c r="D4" s="14" t="n">
-        <v>5000</v>
+        <v>5500</v>
       </c>
       <c r="E4" s="14" t="n">
-        <v>5000</v>
+        <v>5500</v>
       </c>
       <c r="F4" s="14" t="n">
-        <v>5000</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="6" t="inlineStr">
         <is>
-          <t>月間利用回数</t>
+          <t>頻度/回数（月間）</t>
         </is>
       </c>
       <c r="B5" s="14" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" s="14" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D5" s="14" t="n">
         <v>4</v>
@@ -990,7 +990,7 @@
     <row r="6">
       <c r="A6" s="6" t="inlineStr">
         <is>
-          <t>解約率（月次）</t>
+          <t>成長率/解約率</t>
         </is>
       </c>
       <c r="B6" s="15" t="n">
@@ -1063,33 +1063,7 @@
         <v/>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="6" t="inlineStr">
-        <is>
-          <t>LTV</t>
-        </is>
-      </c>
-      <c r="B9" s="7">
-        <f>IF(B6=0,0,B4/B6)</f>
-        <v/>
-      </c>
-      <c r="C9" s="7">
-        <f>IF(C6=0,0,C4/C6)</f>
-        <v/>
-      </c>
-      <c r="D9" s="7">
-        <f>IF(D6=0,0,D4/D6)</f>
-        <v/>
-      </c>
-      <c r="E9" s="7">
-        <f>IF(E6=0,0,E4/E6)</f>
-        <v/>
-      </c>
-      <c r="F9" s="7">
-        <f>IF(F6=0,0,F4/F6)</f>
-        <v/>
-      </c>
-    </row>
+    <row r="9" ht="6" customHeight="1"/>
     <row r="10">
       <c r="A10" s="11" t="inlineStr">
         <is>
@@ -1150,7 +1124,7 @@
     <row r="1" ht="30" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>アカデミーモデル（教育事業）</t>
+          <t>収益モデル2（セグメント2）</t>
         </is>
       </c>
     </row>
@@ -1185,64 +1159,64 @@
     <row r="3">
       <c r="A3" s="6" t="inlineStr">
         <is>
-          <t>受講者数</t>
+          <t>顧客数/取引数</t>
         </is>
       </c>
       <c r="B3" s="14" t="n">
-        <v>30</v>
+        <v>75</v>
       </c>
       <c r="C3" s="14" t="n">
-        <v>60</v>
+        <v>150</v>
       </c>
       <c r="D3" s="14" t="n">
-        <v>100</v>
+        <v>270</v>
       </c>
       <c r="E3" s="14" t="n">
-        <v>160</v>
+        <v>420</v>
       </c>
       <c r="F3" s="14" t="n">
-        <v>250</v>
+        <v>600</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="6" t="inlineStr">
         <is>
-          <t>講座単価</t>
+          <t>単価（円）</t>
         </is>
       </c>
       <c r="B4" s="14" t="n">
-        <v>30000</v>
+        <v>10000</v>
       </c>
       <c r="C4" s="14" t="n">
-        <v>30000</v>
+        <v>10000</v>
       </c>
       <c r="D4" s="14" t="n">
-        <v>32000</v>
+        <v>10500</v>
       </c>
       <c r="E4" s="14" t="n">
-        <v>32000</v>
+        <v>10500</v>
       </c>
       <c r="F4" s="14" t="n">
-        <v>35000</v>
+        <v>11000</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="6" t="inlineStr">
         <is>
-          <t>開催回数/月</t>
+          <t>頻度/回数（月間）</t>
         </is>
       </c>
       <c r="B5" s="14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C5" s="14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D5" s="14" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E5" s="14" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F5" s="14" t="n">
         <v>4</v>
@@ -1251,23 +1225,23 @@
     <row r="6">
       <c r="A6" s="6" t="inlineStr">
         <is>
-          <t>コンテンツ数</t>
-        </is>
-      </c>
-      <c r="B6" s="14" t="n">
-        <v>5</v>
-      </c>
-      <c r="C6" s="14" t="n">
-        <v>10</v>
-      </c>
-      <c r="D6" s="14" t="n">
-        <v>18</v>
-      </c>
-      <c r="E6" s="14" t="n">
-        <v>25</v>
-      </c>
-      <c r="F6" s="14" t="n">
-        <v>35</v>
+          <t>成長率/解約率</t>
+        </is>
+      </c>
+      <c r="B6" s="15" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="C6" s="15" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="D6" s="15" t="n">
+        <v>0.025</v>
+      </c>
+      <c r="E6" s="15" t="n">
+        <v>0.025</v>
+      </c>
+      <c r="F6" s="15" t="n">
+        <v>0.02</v>
       </c>
     </row>
     <row r="7">
@@ -1324,6 +1298,7 @@
         <v/>
       </c>
     </row>
+    <row r="9" ht="6" customHeight="1"/>
     <row r="10">
       <c r="A10" s="11" t="inlineStr">
         <is>
@@ -1373,7 +1348,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="26" customWidth="1" min="1" max="1"/>
+    <col width="24" customWidth="1" min="1" max="1"/>
     <col width="16" customWidth="1" min="2" max="2"/>
     <col width="16" customWidth="1" min="3" max="3"/>
     <col width="16" customWidth="1" min="4" max="4"/>
@@ -1384,7 +1359,7 @@
     <row r="1" ht="30" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>コンサルモデル（フライホイール）</t>
+          <t>収益モデル3（セグメント3）</t>
         </is>
       </c>
     </row>
@@ -1419,89 +1394,89 @@
     <row r="3">
       <c r="A3" s="6" t="inlineStr">
         <is>
-          <t>コンサルタント数</t>
+          <t>顧客数/取引数</t>
         </is>
       </c>
       <c r="B3" s="14" t="n">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="C3" s="14" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="D3" s="14" t="n">
-        <v>8</v>
+        <v>180</v>
       </c>
       <c r="E3" s="14" t="n">
-        <v>12</v>
+        <v>280</v>
       </c>
       <c r="F3" s="14" t="n">
-        <v>18</v>
+        <v>400</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="6" t="inlineStr">
         <is>
-          <t>月間案件数/人</t>
+          <t>単価（円）</t>
         </is>
       </c>
       <c r="B4" s="14" t="n">
-        <v>2</v>
+        <v>15000</v>
       </c>
       <c r="C4" s="14" t="n">
-        <v>2</v>
+        <v>15000</v>
       </c>
       <c r="D4" s="14" t="n">
-        <v>3</v>
+        <v>15500</v>
       </c>
       <c r="E4" s="14" t="n">
-        <v>3</v>
+        <v>15500</v>
       </c>
       <c r="F4" s="14" t="n">
-        <v>3</v>
+        <v>16000</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="6" t="inlineStr">
         <is>
-          <t>案件単価</t>
+          <t>頻度/回数（月間）</t>
         </is>
       </c>
       <c r="B5" s="14" t="n">
-        <v>500000</v>
+        <v>3</v>
       </c>
       <c r="C5" s="14" t="n">
-        <v>500000</v>
+        <v>3</v>
       </c>
       <c r="D5" s="14" t="n">
-        <v>600000</v>
+        <v>4</v>
       </c>
       <c r="E5" s="14" t="n">
-        <v>600000</v>
+        <v>4</v>
       </c>
       <c r="F5" s="14" t="n">
-        <v>700000</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="6" t="inlineStr">
         <is>
-          <t>稼働率</t>
+          <t>成長率/解約率</t>
         </is>
       </c>
       <c r="B6" s="15" t="n">
-        <v>0.7</v>
+        <v>0.03</v>
       </c>
       <c r="C6" s="15" t="n">
-        <v>0.75</v>
+        <v>0.03</v>
       </c>
       <c r="D6" s="15" t="n">
-        <v>0.8</v>
+        <v>0.025</v>
       </c>
       <c r="E6" s="15" t="n">
-        <v>0.85</v>
+        <v>0.025</v>
       </c>
       <c r="F6" s="15" t="n">
-        <v>0.85</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="7">
@@ -1511,23 +1486,23 @@
         </is>
       </c>
       <c r="B7" s="7">
-        <f>B3*B4*B5*B6</f>
+        <f>B3*B4</f>
         <v/>
       </c>
       <c r="C7" s="7">
-        <f>C3*C4*C5*C6</f>
+        <f>C3*C4</f>
         <v/>
       </c>
       <c r="D7" s="7">
-        <f>D3*D4*D5*D6</f>
+        <f>D3*D4</f>
         <v/>
       </c>
       <c r="E7" s="7">
-        <f>E3*E4*E5*E6</f>
+        <f>E3*E4</f>
         <v/>
       </c>
       <c r="F7" s="7">
-        <f>F3*F4*F5*F6</f>
+        <f>F3*F4</f>
         <v/>
       </c>
     </row>
@@ -1558,6 +1533,7 @@
         <v/>
       </c>
     </row>
+    <row r="9" ht="6" customHeight="1"/>
     <row r="10">
       <c r="A10" s="11" t="inlineStr">
         <is>
@@ -2835,7 +2811,7 @@
       </c>
       <c r="C3" s="23" t="inlineStr">
         <is>
-          <t>ヘルスケア×教育市場</t>
+          <t>対象市場全体</t>
         </is>
       </c>
     </row>
@@ -2920,7 +2896,7 @@
       </c>
       <c r="C8" s="23" t="inlineStr">
         <is>
-          <t>食材・講師・外注費</t>
+          <t>変動費ベース</t>
         </is>
       </c>
     </row>

</xml_diff>